<commit_message>
IMP:Add Field Track2 In Report GL Summary
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_gl_summary.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_gl_summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>General Ledger [Summary]</t>
   </si>
@@ -29,10 +29,16 @@
     <t>{{#if track_name}}</t>
   </si>
   <si>
-    <t>Tracking: {{track_name}}</t>
+    <t>Tracking-1: {{track_name}}</t>
   </si>
   <si>
     <t>{{/if}}</t>
+  </si>
+  <si>
+    <t>{{#if track2_name}}</t>
+  </si>
+  <si>
+    <t>Tracking-2: {{track2_name}}</t>
   </si>
   <si>
     <t>Account</t>
@@ -85,7 +91,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -121,12 +127,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF800000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -206,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -235,15 +235,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,15 +247,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -280,10 +276,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -343,70 +339,97 @@
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" s="8" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="10" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C13" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="12" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="12" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="C15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>